<commit_message>
New script + New study
</commit_message>
<xml_diff>
--- a/spec/init_database_table_ppl.xlsx
+++ b/spec/init_database_table_ppl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chloe\Documents\projets-csd\250422_appli_scripts\spec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chloe\SNDSQueryHub\spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3538F3-B9F8-47D0-8328-81DAA4A0E1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4DD22A-20E6-4706-9F3F-28D1FCC3789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="550" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{11FCEF69-134C-4E2B-AFC9-F109D8E49774}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{11FCEF69-134C-4E2B-AFC9-F109D8E49774}"/>
   </bookViews>
   <sheets>
     <sheet name="script" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>script_id</t>
   </si>
@@ -110,18 +110,12 @@
     <t>study_description</t>
   </si>
   <si>
-    <t xml:space="preserve">Adherence to Antidepressant Initiation Guidelines Over 10 Years: A French National Retrospective Study </t>
-  </si>
-  <si>
     <t>Chloé Saint-Dizier</t>
   </si>
   <si>
     <t>Variations in Dispensing Psychotropic Drugs to Adolescents Depending on School Periods: A French Nationwide Retrospective Study</t>
   </si>
   <si>
-    <t>L’étude décrit les séquences de traitement par antidépresseurs avec un suivi de 2 ans dans le cadre d’un premier épisode dépressif entre 2017 et 2021, ainsi que leur conformité aux recommandations de la Haute Autorité de Santé. Une comparaison est réalisée entre les patients suivis uniquement par leur médecin généraliste et ceux ayant reçu au moins une prescription d’antidépresseur de la part d’un psychiatre au cours de leur séquence de traitement.</t>
-  </si>
-  <si>
     <t>script_id_required</t>
   </si>
   <si>
@@ -147,6 +141,36 @@
   </si>
   <si>
     <t>../scripts/R/inclusion_sequences.R</t>
+  </si>
+  <si>
+    <t>inclusion_sej_mco_par_diag.R</t>
+  </si>
+  <si>
+    <t>../scripts/R/inclusion_sej_mco_par_diag.R</t>
+  </si>
+  <si>
+    <t>Inclure tous les séjours en MCO avec un ou plusieurs diagnostics sur plusieurs années</t>
+  </si>
+  <si>
+    <t>Inclusion de séjours en MCO par les diagnostics</t>
+  </si>
+  <si>
+    <t>Aurélie Lescroart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respect des recommandations de primo-prescription des antidépresseurs en France : étude rétrospective observationnelle à partir du SNDS entre 2012 et 2022 </t>
+  </si>
+  <si>
+    <t>L’étude décrit les séquences de traitement par antidépresseurs avec un suivi de 2 ans dans le cadre d’un premier épisode dépressif entre 2012 et 2022, ainsi que leur conformité aux recommandations de la Haute Autorité de Santé. Une comparaison est réalisée entre les patients suivis uniquement par leur médecin généraliste et ceux ayant reçu au moins une prescription d’antidépresseur de la part d’un psychiatre au cours de leur séquence de traitement.</t>
+  </si>
+  <si>
+    <t>Mortalité chez les patients catatoniques</t>
+  </si>
+  <si>
+    <t>Ali Amad</t>
+  </si>
+  <si>
+    <t>L'objectif principale de l'étude est de décrire la mortalité chez les patients catatoniques avec une analyse de survie. L'objectif secondaire est d'évaluer l'impact de l'ECT sur ette mortalité.</t>
   </si>
 </sst>
 </file>
@@ -527,15 +551,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CD28CE-642D-45CF-995E-76D8D5434FE6}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -578,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>7</v>
@@ -607,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -619,7 +646,7 @@
         <v>45755</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -636,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -648,9 +675,38 @@
         <v>45756</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45828</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -661,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86D47E4-922F-46A2-B750-46298F58E64A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -697,22 +753,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>5</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -720,10 +776,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1">
         <v>45776</v>
@@ -735,7 +791,30 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45828</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -745,10 +824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D212A8-7F8F-47A4-BACA-19F1F454559A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +842,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -771,7 +850,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -779,26 +858,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -808,10 +879,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57860B64-6C89-40A5-A081-2DD0919FB406}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -837,6 +908,14 @@
         <v>3</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
     </row>

</xml_diff>